<commit_message>
added more cues and track nums
</commit_message>
<xml_diff>
--- a/Audio/Russman/cues.xlsx
+++ b/Audio/Russman/cues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fifem\Documents\drg-mods\Audio\Russman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF9ABA9-7505-454E-BF0C-B79B3A1440FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6532C791-F60B-4695-B5B2-D78B14D2786C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10920" windowHeight="7428" xr2:uid="{F8A3E8D9-1FAC-42EC-8E85-BA0F2CBBD7A8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Description</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Shout_EnvironmentSnowStorm</t>
   </si>
   <si>
-    <t>got a bad feeling about this storm</t>
-  </si>
-  <si>
     <t>out of money</t>
   </si>
   <si>
@@ -118,6 +115,114 @@
   </si>
   <si>
     <t>get it off</t>
+  </si>
+  <si>
+    <t>Russman Track #</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>01, 03, 07, 08, 09</t>
+  </si>
+  <si>
+    <t>46, 47</t>
+  </si>
+  <si>
+    <t>77, 78</t>
+  </si>
+  <si>
+    <t>Shouts/Mission_Escort/</t>
+  </si>
+  <si>
+    <t>Shout_ProtectDrilldozer_WhenTakingDamage</t>
+  </si>
+  <si>
+    <t>Shout_AfterDrilldozerStarted_Firsttime</t>
+  </si>
+  <si>
+    <t>89, 90, 98, 99</t>
+  </si>
+  <si>
+    <t>132, 135</t>
+  </si>
+  <si>
+    <t>137, 138, 139</t>
+  </si>
+  <si>
+    <t>Shout_PickAxePowerAttack</t>
+  </si>
+  <si>
+    <t>241, 242, 243, 244, 245, 246, 247, 248</t>
+  </si>
+  <si>
+    <t>grenade kill</t>
+  </si>
+  <si>
+    <t>251, 253</t>
+  </si>
+  <si>
+    <t>277, 289, 290, 291, 293</t>
+  </si>
+  <si>
+    <t>getting fuel</t>
+  </si>
+  <si>
+    <t>Shout_CanisterFull</t>
+  </si>
+  <si>
+    <t>wave incoming</t>
+  </si>
+  <si>
+    <t>tunnels…</t>
+  </si>
+  <si>
+    <t>leaving mission</t>
+  </si>
+  <si>
+    <t>Shout_Environment_HeavyRainFall</t>
+  </si>
+  <si>
+    <t>smell</t>
+  </si>
+  <si>
+    <t>345, 349, 354</t>
+  </si>
+  <si>
+    <t>mission fail</t>
+  </si>
+  <si>
+    <t>359, 360, 361, 362</t>
+  </si>
+  <si>
+    <t>149, 150, 151, 152, 369</t>
+  </si>
+  <si>
+    <t>24, 207, 209, 210, 211, 370, 372</t>
+  </si>
+  <si>
+    <t>333, 374, 377, 379, 380</t>
+  </si>
+  <si>
+    <t>Shout_Minerals_Buy</t>
+  </si>
+  <si>
+    <t>Shout_Minerals_GoodDeal</t>
+  </si>
+  <si>
+    <t>Shout_Minerals_Sell</t>
+  </si>
+  <si>
+    <t>Shout_FlyingGrabber</t>
+  </si>
+  <si>
+    <t>Shout_LightUp</t>
+  </si>
+  <si>
+    <t>Shouts/LaserPointer/</t>
+  </si>
+  <si>
+    <t>Shout_LaserPoint_Generic</t>
   </si>
 </sst>
 </file>
@@ -161,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -174,6 +279,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,196 +599,393 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6AF122-86AA-492E-835B-7E2AA6F17D7A}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B17:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.109375" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2">
         <v>0.34166666666666662</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="2">
         <v>0.42708333333333331</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6">
+        <v>280</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B14" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2">
         <v>0.12638888888888888</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.58750000000000002</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="2">
         <v>0.20833333333333334</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="6">
+        <v>320</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="6">
+        <v>351</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="6">
+        <v>13</v>
+      </c>
+      <c r="C30" s="9">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="6">
+        <v>13</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B32" s="6">
+        <v>129</v>
+      </c>
+      <c r="C32" s="2">
         <v>0.33819444444444446</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D32" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="3">
-        <v>3.8194444444444441E-2</v>
-      </c>
-      <c r="C20" s="4" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.33888888888888885</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.81597222222222221</v>
+      </c>
+      <c r="D41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0.33888888888888885</v>
-      </c>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="2">
-        <v>0.81597222222222221</v>
-      </c>
-      <c r="C26" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C42" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="s">
+      <c r="D42" t="s">
         <v>29</v>
       </c>
-      <c r="C27" t="s">
-        <v>30</v>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="6">
+        <v>340</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="6">
+        <v>352</v>
+      </c>
+      <c r="D47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="6">
+        <v>358</v>
+      </c>
+      <c r="D48" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-  </mergeCells>
+  <sortState ref="A29:D36">
+    <sortCondition ref="A29:A36"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some more cues
</commit_message>
<xml_diff>
--- a/Audio/Russman/cues.xlsx
+++ b/Audio/Russman/cues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fifem\Documents\drg-mods\Audio\Russman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6532C791-F60B-4695-B5B2-D78B14D2786C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6938880-16A7-4D99-B7EB-D266BA214F4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10920" windowHeight="7428" xr2:uid="{F8A3E8D9-1FAC-42EC-8E85-BA0F2CBBD7A8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Description</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Shout_Grenade_Warning_Lure</t>
   </si>
   <si>
-    <t>Monkey bomb</t>
-  </si>
-  <si>
     <t>Shout_EnvironmentSandstorm</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>Shout_AfterDrilldozerStarted_Firsttime</t>
   </si>
   <si>
-    <t>89, 90, 98, 99</t>
-  </si>
-  <si>
     <t>132, 135</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>Shout_PickAxePowerAttack</t>
   </si>
   <si>
-    <t>241, 242, 243, 244, 245, 246, 247, 248</t>
-  </si>
-  <si>
     <t>grenade kill</t>
   </si>
   <si>
@@ -223,6 +214,33 @@
   </si>
   <si>
     <t>Shout_LaserPoint_Generic</t>
+  </si>
+  <si>
+    <t>15, 280</t>
+  </si>
+  <si>
+    <t>39, 241, 242, 243, 244, 245, 246, 247, 248</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>ought to be able to do something with this</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>can't keep hauling this around</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>89, 90, 97, 98, 99, 100</t>
   </si>
 </sst>
 </file>
@@ -599,11 +617,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6AF122-86AA-492E-835B-7E2AA6F17D7A}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B17:B18"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,7 +638,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -634,7 +652,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2">
         <v>0.34166666666666662</v>
@@ -645,12 +663,15 @@
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>59</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -663,7 +684,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -671,7 +692,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2">
         <v>0.42708333333333331</v>
@@ -679,10 +700,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -696,19 +717,16 @@
       <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="6">
-        <v>280</v>
+      <c r="B11" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C11" s="2">
         <v>0.58750000000000002</v>
       </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -717,7 +735,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2">
         <v>1.3888888888888888E-2</v>
@@ -728,7 +746,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -736,7 +754,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="2">
         <v>0.12638888888888888</v>
@@ -750,12 +768,15 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>65</v>
       </c>
       <c r="C18" s="2"/>
@@ -771,7 +792,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2">
         <v>0.20833333333333334</v>
@@ -785,13 +806,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="6">
         <v>112</v>
@@ -799,21 +820,21 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B25" s="6">
         <v>320</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -824,7 +845,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B29" s="6">
         <v>351</v>
@@ -834,7 +855,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="6">
         <v>13</v>
@@ -846,7 +867,7 @@
     </row>
     <row r="31" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="6">
         <v>13</v>
@@ -870,21 +891,21 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="4"/>
@@ -905,7 +926,7 @@
         <v>21</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C39" s="2">
         <v>0.33888888888888885</v>
@@ -916,37 +937,37 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C41" s="2">
         <v>0.81597222222222221</v>
       </c>
       <c r="D41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" t="s">
         <v>28</v>
-      </c>
-      <c r="D42" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D43" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -954,15 +975,15 @@
         <v>340</v>
       </c>
       <c r="D45" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B46" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -970,7 +991,7 @@
         <v>352</v>
       </c>
       <c r="D47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -978,7 +999,23 @@
         <v>358</v>
       </c>
       <c r="D48" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added out-of-grenades voice line
</commit_message>
<xml_diff>
--- a/Audio/Russman/cues.xlsx
+++ b/Audio/Russman/cues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fifem\Documents\drg-mods\Audio\Russman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA865F38-0D68-4793-B1BD-E9205150D317}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3642C503-75F7-4DD7-8FB1-23B4DB1D3662}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10920" windowHeight="7428" xr2:uid="{F8A3E8D9-1FAC-42EC-8E85-BA0F2CBBD7A8}"/>
   </bookViews>
@@ -626,7 +626,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,7 +737,7 @@
       <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented sentry build lines
</commit_message>
<xml_diff>
--- a/Audio/Russman/cues.xlsx
+++ b/Audio/Russman/cues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fifem\Documents\drg-mods\Audio\Russman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3642C503-75F7-4DD7-8FB1-23B4DB1D3662}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E705CAB-D301-42B2-A46A-DF57294CD0EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10920" windowHeight="7428" xr2:uid="{F8A3E8D9-1FAC-42EC-8E85-BA0F2CBBD7A8}"/>
   </bookViews>
@@ -626,7 +626,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,7 +745,7 @@
       <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D15" t="s">

</xml_diff>

<commit_message>
transitioned to shout framework and implemented out-of-ammo shout
</commit_message>
<xml_diff>
--- a/Audio/Russman/cues.xlsx
+++ b/Audio/Russman/cues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fifem\Documents\drg-mods\Audio\Russman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E705CAB-D301-42B2-A46A-DF57294CD0EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3248351B-3EE6-4A87-B355-AD466326E2A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10920" windowHeight="7428" xr2:uid="{F8A3E8D9-1FAC-42EC-8E85-BA0F2CBBD7A8}"/>
   </bookViews>
@@ -261,18 +261,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -299,20 +293,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -626,7 +612,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,7 +715,7 @@
       <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>28</v>
       </c>
     </row>
@@ -737,7 +723,7 @@
       <c r="A14" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -745,7 +731,7 @@
       <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D15" t="s">
@@ -984,11 +970,6 @@
   <sortState ref="A29:D36">
     <sortCondition ref="A29:A36"/>
   </sortState>
-  <conditionalFormatting sqref="B2:B39">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B2))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>